<commit_message>
"Added codes split to calculate the features across & Features calculations"
</commit_message>
<xml_diff>
--- a/AML_Feature_Calculations.xlsx
+++ b/AML_Feature_Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc4bd521ffc22738/Desktop/Freelancing/AIGEN/smartsentry_aml_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D1C74165-A2F8-4269-86D0-126BC9A44AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFD6917D-FFE8-439A-88E0-E0A1AEE23D2F}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{D1C74165-A2F8-4269-86D0-126BC9A44AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{455AF32B-E2CF-4507-8950-E4D6B5AD88C3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="393">
   <si>
     <t>SmartSentry AML — New Feature Calculations Reference</t>
   </si>
@@ -297,9 +297,6 @@
   </si>
   <si>
     <t>debit</t>
-  </si>
-  <si>
-    <t>₹22,026 (avg_balance — 1st txn)</t>
   </si>
   <si>
     <t>−₹12,000</t>
@@ -1220,6 +1217,9 @@
   </si>
   <si>
     <t>Graph edge: email_group → N customer nodes</t>
+  </si>
+  <si>
+    <t>₹70,000 (avg_balance — 1st txn)</t>
   </si>
 </sst>
 </file>
@@ -1623,24 +1623,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1650,38 +1650,38 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1766,6 +1766,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2412,11 +2416,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2425,23 +2429,24 @@
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="6" width="28" customWidth="1"/>
-    <col min="7" max="8" width="36" customWidth="1"/>
+    <col min="5" max="7" width="28" customWidth="1"/>
+    <col min="8" max="9" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-    </row>
-    <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+    </row>
+    <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>76</v>
       </c>
@@ -2452,8 +2457,9 @@
       <c r="F2" s="39"/>
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
-    </row>
-    <row r="3" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>77</v>
       </c>
@@ -2473,13 +2479,16 @@
         <v>65</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>82</v>
       </c>
@@ -2493,247 +2502,274 @@
         <v>85</v>
       </c>
       <c r="E4" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="G4" s="18">
+        <f>70000-12000</f>
+        <v>58000</v>
+      </c>
+      <c r="H4" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="I4" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" s="19">
+        <f>G4+C5</f>
+        <v>61500</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="18">
+        <f>G5-C6</f>
+        <v>53500</v>
+      </c>
+      <c r="H6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="I6" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="19">
+        <f>G6-C7</f>
+        <v>28500</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="I7" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="19" t="s">
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="18" t="s">
+      <c r="F8" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>112</v>
+      <c r="G8" s="18">
+        <f>G7+C8</f>
+        <v>33500</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="I8" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+    </row>
+    <row r="11" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="B11" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="H11" s="43"/>
-    </row>
-    <row r="12" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="41"/>
+    </row>
+    <row r="12" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="H12" s="45"/>
-    </row>
-    <row r="13" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="43"/>
+    </row>
+    <row r="13" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="H13" s="43"/>
-    </row>
-    <row r="14" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="41"/>
+    </row>
+    <row r="14" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="H14" s="45"/>
-    </row>
-    <row r="15" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="43"/>
+    </row>
+    <row r="15" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="H15" s="43"/>
-    </row>
-    <row r="16" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="41"/>
+    </row>
+    <row r="16" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="H16" s="45"/>
+      <c r="I16" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="B15:F15"/>
-    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="B16:F16"/>
-    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="H12:I12"/>
     <mergeCell ref="B13:F13"/>
-    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="H13:I13"/>
     <mergeCell ref="B14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2745,7 +2781,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D12" sqref="D12:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2760,7 +2796,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -2770,7 +2806,7 @@
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="47"/>
       <c r="C2" s="47"/>
@@ -2780,87 +2816,87 @@
     </row>
     <row r="3" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
@@ -2870,161 +2906,161 @@
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
@@ -3034,71 +3070,71 @@
     </row>
     <row r="20" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3117,15 +3153,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" activeCellId="2" sqref="A3:B11 E3:E11 G3:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.5546875" customWidth="1"/>
     <col min="2" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
     <col min="7" max="7" width="39.44140625" customWidth="1"/>
@@ -3134,7 +3170,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -3145,7 +3181,7 @@
     </row>
     <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
@@ -3159,22 +3195,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -3182,22 +3218,22 @@
         <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -3205,22 +3241,22 @@
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -3228,22 +3264,22 @@
         <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -3251,22 +3287,22 @@
         <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -3274,22 +3310,22 @@
         <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -3297,22 +3333,22 @@
         <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -3320,22 +3356,22 @@
         <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -3343,35 +3379,35 @@
         <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3379,10 +3415,10 @@
         <v>48</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>249</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>78</v>
@@ -3399,71 +3435,71 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G15" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>260</v>
-      </c>
       <c r="G16" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>264</v>
-      </c>
       <c r="G17" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3496,7 +3532,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -3505,113 +3541,113 @@
       <c r="F1" s="46"/>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="A2" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>269</v>
-      </c>
       <c r="F3" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -3619,70 +3655,70 @@
         <v>71</v>
       </c>
       <c r="B8" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="D8" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="E8" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="F8" s="24" t="s">
         <v>295</v>
       </c>
-      <c r="F8" s="24" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="45" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+    </row>
+    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="56" t="s">
         <v>297</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-    </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50" t="s">
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+    </row>
+    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-    </row>
-    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50" t="s">
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+    </row>
+    <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45" t="s">
         <v>299</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-    </row>
-    <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
-        <v>300</v>
-      </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
     </row>
     <row r="15" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>303</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -3690,206 +3726,211 @@
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="C16" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="C16" s="53" t="s">
-        <v>306</v>
-      </c>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
     </row>
     <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="C17" s="52" t="s">
         <v>308</v>
       </c>
-      <c r="C17" s="54" t="s">
-        <v>309</v>
-      </c>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="B18" s="30" t="s">
         <v>310</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="C18" s="53" t="s">
         <v>311</v>
       </c>
-      <c r="C18" s="55" t="s">
-        <v>312</v>
-      </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
     </row>
     <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="B19" s="32" t="s">
         <v>313</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="C19" s="54" t="s">
         <v>314</v>
       </c>
-      <c r="C19" s="56" t="s">
-        <v>315</v>
-      </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
     </row>
     <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>316</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="C20" s="49" t="s">
         <v>317</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+    </row>
+    <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="50" t="s">
         <v>318</v>
       </c>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-    </row>
-    <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52" t="s">
-        <v>319</v>
-      </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
     </row>
     <row r="23" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>321</v>
-      </c>
       <c r="D23" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>71</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E24" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="8" t="s">
         <v>327</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="E25" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>332</v>
-      </c>
       <c r="F25" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="8" t="s">
         <v>337</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="C27" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>342</v>
-      </c>
       <c r="F27" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="E28" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>347</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A14:F14"/>
@@ -3897,11 +3938,6 @@
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3928,7 +3964,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -3937,33 +3973,33 @@
       <c r="F1" s="46"/>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
-        <v>349</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="A2" s="59" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
     </row>
     <row r="3" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>354</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3971,19 +4007,19 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>359</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3991,19 +4027,19 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4011,34 +4047,34 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="F6" s="3" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="59" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
-        <v>369</v>
-      </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="58" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B9" s="58"/>
       <c r="C9" s="58"/>
@@ -4047,18 +4083,18 @@
       <c r="F9" s="58"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="59" t="s">
-        <v>371</v>
-      </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
+      <c r="A10" s="57" t="s">
+        <v>370</v>
+      </c>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B11" s="58"/>
       <c r="C11" s="58"/>
@@ -4067,18 +4103,18 @@
       <c r="F11" s="58"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59" t="s">
-        <v>373</v>
-      </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
+      <c r="A12" s="57" t="s">
+        <v>372</v>
+      </c>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="58" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B13" s="58"/>
       <c r="C13" s="58"/>
@@ -4087,18 +4123,18 @@
       <c r="F13" s="58"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="59" t="s">
-        <v>375</v>
-      </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
+      <c r="A14" s="57" t="s">
+        <v>374</v>
+      </c>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="58" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B15" s="58"/>
       <c r="C15" s="58"/>
@@ -4107,18 +4143,18 @@
       <c r="F15" s="58"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="59" t="s">
-        <v>377</v>
-      </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
+      <c r="A16" s="57" t="s">
+        <v>376</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="58" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B17" s="58"/>
       <c r="C17" s="58"/>
@@ -4127,37 +4163,37 @@
       <c r="F17" s="58"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="57" t="s">
+        <v>378</v>
+      </c>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+    </row>
+    <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="45" t="s">
         <v>379</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-    </row>
-    <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="41" t="s">
-        <v>380</v>
-      </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
     </row>
     <row r="21" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>382</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>383</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -4167,51 +4203,61 @@
         <v>9</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="41" t="s">
         <v>385</v>
       </c>
-      <c r="D22" s="43" t="s">
-        <v>386</v>
-      </c>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="43" t="s">
         <v>388</v>
       </c>
-      <c r="D23" s="45" t="s">
-        <v>389</v>
-      </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
     </row>
     <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="41" t="s">
         <v>391</v>
       </c>
-      <c r="D24" s="43" t="s">
-        <v>392</v>
-      </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="A16:F16"/>
@@ -4219,16 +4265,6 @@
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="D22:F22"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>